<commit_message>
big update: - generated reviews - generated webstats - modularized everything
</commit_message>
<xml_diff>
--- a/data_new/newEmployees.xlsx
+++ b/data_new/newEmployees.xlsx
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>32263</v>
+        <v>32265</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>44563</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>37405</v>
+        <v>37407</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>44564</v>
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>30509</v>
+        <v>30511</v>
       </c>
       <c r="I4" s="3" t="n">
         <v>44562</v>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>31844</v>
+        <v>31846</v>
       </c>
       <c r="I5" s="3" t="n">
         <v>44565</v>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>38003</v>
+        <v>38005</v>
       </c>
       <c r="I6" s="3" t="n">
         <v>44565</v>
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>28490</v>
+        <v>28492</v>
       </c>
       <c r="I7" s="3" t="n">
         <v>44565</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>34969</v>
+        <v>34971</v>
       </c>
       <c r="I8" s="3" t="n">
         <v>44929</v>
@@ -813,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>28127</v>
+        <v>28129</v>
       </c>
       <c r="I9" s="3" t="n">
         <v>44928</v>
@@ -854,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>29504</v>
+        <v>29506</v>
       </c>
       <c r="I10" s="3" t="n">
         <v>44927</v>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>36333</v>
+        <v>36335</v>
       </c>
       <c r="I11" s="3" t="n">
         <v>44930</v>
@@ -936,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>31286</v>
+        <v>31288</v>
       </c>
       <c r="I12" s="3" t="n">
         <v>44929</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>37171</v>
+        <v>37173</v>
       </c>
       <c r="I13" s="3" t="n">
         <v>44927</v>
@@ -1018,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>36452</v>
+        <v>36454</v>
       </c>
       <c r="I14" s="3" t="n">
         <v>44930</v>
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>34237</v>
+        <v>34239</v>
       </c>
       <c r="I15" s="3" t="n">
         <v>44929</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>31806</v>
+        <v>31808</v>
       </c>
       <c r="I16" s="3" t="n">
         <v>44929</v>
@@ -1141,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>27668</v>
+        <v>27670</v>
       </c>
       <c r="I17" s="3" t="n">
         <v>45294</v>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>36810</v>
+        <v>36812</v>
       </c>
       <c r="I18" s="3" t="n">
         <v>45294</v>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>37550</v>
+        <v>37552</v>
       </c>
       <c r="I19" s="3" t="n">
         <v>45293</v>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>29855</v>
+        <v>29857</v>
       </c>
       <c r="I20" s="3" t="n">
         <v>45294</v>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>33042</v>
+        <v>33044</v>
       </c>
       <c r="I21" s="3" t="n">
         <v>45294</v>
@@ -1346,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>30119</v>
+        <v>30121</v>
       </c>
       <c r="I22" s="3" t="n">
         <v>45295</v>
@@ -1387,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>33399</v>
+        <v>33401</v>
       </c>
       <c r="I23" s="3" t="n">
         <v>45658</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>29655</v>
+        <v>29657</v>
       </c>
       <c r="I24" s="3" t="n">
         <v>45661</v>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>30742</v>
+        <v>30744</v>
       </c>
       <c r="I25" s="3" t="n">
         <v>45661</v>
@@ -1510,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>34580</v>
+        <v>34582</v>
       </c>
       <c r="I26" s="3" t="n">
         <v>45659</v>
@@ -1551,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>31379</v>
+        <v>31381</v>
       </c>
       <c r="I27" s="3" t="n">
         <v>45661</v>

</xml_diff>